<commit_message>
accessing and writing into excel files using openpyxl
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bishal\OneDrive\Desktop\python-for-devops\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1E8ED4-A52F-4951-9423-A22214B35CCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -37,26 +46,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -64,7 +79,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -74,41 +89,42 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -298,23 +314,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:G75"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="4" max="4" width="14.86"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -328,12 +349,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
         <v>200.4</v>
@@ -343,26 +364,26 @@
       </c>
       <c r="G2" s="4"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="2">
-        <v>30000.0</v>
+        <v>30000</v>
       </c>
       <c r="C4" s="2">
         <v>234.99</v>
@@ -371,12 +392,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2">
         <v>21.89</v>
@@ -385,12 +406,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>523.0</v>
+        <v>523</v>
       </c>
       <c r="C6" s="2">
         <v>55.99</v>
@@ -399,26 +420,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3">
-        <v>1150.0</v>
+        <v>1150</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C8" s="2">
         <v>122.55</v>
@@ -427,26 +448,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>2352.0</v>
+        <v>2352</v>
       </c>
       <c r="C9" s="3">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>666.0</v>
+        <v>666</v>
       </c>
       <c r="C10" s="3">
         <v>345.99</v>
@@ -455,26 +476,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C11" s="3">
-        <v>646.95</v>
+        <v>646.95000000000005</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="C12" s="3">
         <v>13.99</v>
@@ -483,26 +504,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="C13" s="3">
-        <v>2352.55</v>
+        <v>2352.5500000000002</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>458.0</v>
+        <v>458</v>
       </c>
       <c r="C14" s="3">
         <v>324.5</v>
@@ -511,12 +532,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="C15" s="3">
         <v>235.99</v>
@@ -525,12 +546,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>535.0</v>
+        <v>535</v>
       </c>
       <c r="C16" s="3">
         <v>235.98</v>
@@ -539,12 +560,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C17" s="3">
         <v>9.99</v>
@@ -553,26 +574,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2">
-        <v>688.0</v>
+        <v>688</v>
       </c>
       <c r="C18" s="3">
-        <v>19.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="C19" s="3">
         <v>24.9</v>
@@ -581,12 +602,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C20" s="3">
         <v>49.5</v>
@@ -595,12 +616,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2">
-        <v>457.0</v>
+        <v>457</v>
       </c>
       <c r="C21" s="2">
         <v>200.4</v>
@@ -609,26 +630,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2">
-        <v>346.0</v>
+        <v>346</v>
       </c>
       <c r="C22" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2">
-        <v>745.0</v>
+        <v>745</v>
       </c>
       <c r="C23" s="2">
         <v>234.99</v>
@@ -637,12 +658,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="C24" s="2">
         <v>21.89</v>
@@ -651,12 +672,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2">
         <v>55.99</v>
@@ -665,26 +686,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="C26" s="2">
-        <v>1150.0</v>
+        <v>1150</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>57346.0</v>
+        <v>57346</v>
       </c>
       <c r="C27" s="2">
         <v>122.55</v>
@@ -693,26 +714,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>743.0</v>
+        <v>743</v>
       </c>
       <c r="C28" s="2">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>364.0</v>
+        <v>364</v>
       </c>
       <c r="C29" s="2">
         <v>345.99</v>
@@ -721,26 +742,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C30" s="2">
-        <v>646.95</v>
+        <v>646.95000000000005</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="C31" s="2">
         <v>13.99</v>
@@ -749,26 +770,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>31.0</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2">
-        <v>2352.55</v>
+        <v>2352.5500000000002</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>32.0</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C33" s="2">
         <v>324.5</v>
@@ -777,12 +798,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C34" s="2">
         <v>235.99</v>
@@ -791,12 +812,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>34.0</v>
+        <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>2352.0</v>
+        <v>2352</v>
       </c>
       <c r="C35" s="2">
         <v>235.98</v>
@@ -805,12 +826,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
-        <v>35.0</v>
+        <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>666.0</v>
+        <v>666</v>
       </c>
       <c r="C36" s="2">
         <v>9.99</v>
@@ -819,26 +840,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>36.0</v>
+        <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C37" s="2">
-        <v>19.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
-        <v>37.0</v>
+        <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="C38" s="2">
         <v>24.9</v>
@@ -847,12 +868,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
-        <v>38.0</v>
+        <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="C39" s="2">
         <v>49.5</v>
@@ -861,12 +882,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
-        <v>39.0</v>
+        <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>458.0</v>
+        <v>458</v>
       </c>
       <c r="C40" s="2">
         <v>200.4</v>
@@ -875,26 +896,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>40.0</v>
+        <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>8567.0</v>
+        <v>8567</v>
       </c>
       <c r="C41" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>41.0</v>
+        <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>535.0</v>
+        <v>535</v>
       </c>
       <c r="C42" s="2">
         <v>234.99</v>
@@ -903,12 +924,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>42.0</v>
+        <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C43" s="2">
         <v>21.89</v>
@@ -917,12 +938,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
-        <v>43.0</v>
+        <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>688.0</v>
+        <v>688</v>
       </c>
       <c r="C44" s="2">
         <v>55.99</v>
@@ -931,26 +952,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>44.0</v>
+        <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="C45" s="2">
-        <v>1150.0</v>
+        <v>1150</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>45.0</v>
+        <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C46" s="2">
         <v>122.55</v>
@@ -959,26 +980,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
-        <v>46.0</v>
+        <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="C47" s="2">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
-        <v>47.0</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="C48" s="2">
         <v>345.99</v>
@@ -987,26 +1008,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
-        <v>48.0</v>
+        <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>458.0</v>
+        <v>458</v>
       </c>
       <c r="C49" s="2">
-        <v>646.95</v>
+        <v>646.95000000000005</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="C50" s="2">
         <v>13.99</v>
@@ -1015,26 +1036,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
-        <v>50.0</v>
+        <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>535.0</v>
+        <v>535</v>
       </c>
       <c r="C51" s="2">
-        <v>2352.55</v>
+        <v>2352.5500000000002</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>51.0</v>
+        <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C52" s="2">
         <v>324.5</v>
@@ -1043,12 +1064,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>688.0</v>
+        <v>688</v>
       </c>
       <c r="C53" s="2">
         <v>235.99</v>
@@ -1057,12 +1078,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
-        <v>53.0</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="C54" s="2">
         <v>24.49</v>
@@ -1071,12 +1092,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C55" s="2">
         <v>9.99</v>
@@ -1085,26 +1106,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C56" s="2">
-        <v>19.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="C57" s="2">
         <v>24.9</v>
@@ -1113,12 +1134,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
-        <v>57.0</v>
+        <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="C58" s="2">
         <v>49.5</v>
@@ -1127,12 +1148,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>458.0</v>
+        <v>458</v>
       </c>
       <c r="C59" s="2">
         <v>200.4</v>
@@ -1141,26 +1162,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="C60" s="2">
-        <v>33.0</v>
+        <v>33</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
-        <v>60.0</v>
+        <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>535.0</v>
+        <v>535</v>
       </c>
       <c r="C61" s="2">
         <v>234.99</v>
@@ -1169,12 +1190,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C62" s="2">
         <v>21.89</v>
@@ -1183,12 +1204,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
-        <v>62.0</v>
+        <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>688.0</v>
+        <v>688</v>
       </c>
       <c r="C63" s="2">
         <v>55.99</v>
@@ -1197,26 +1218,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="C64" s="2">
-        <v>1150.0</v>
+        <v>1150</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>54.0</v>
+        <v>54</v>
       </c>
       <c r="C65" s="2">
         <v>122.55</v>
@@ -1225,26 +1246,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>235.0</v>
+        <v>235</v>
       </c>
       <c r="C66" s="2">
-        <v>111.0</v>
+        <v>111</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
-        <v>66.0</v>
+        <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>77.0</v>
+        <v>77</v>
       </c>
       <c r="C67" s="2">
         <v>345.99</v>
@@ -1253,26 +1274,26 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>85.0</v>
+        <v>85</v>
       </c>
       <c r="C68" s="2">
-        <v>646.95</v>
+        <v>646.95000000000005</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>458.0</v>
+        <v>458</v>
       </c>
       <c r="C69" s="2">
         <v>13.99</v>
@@ -1281,26 +1302,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>234.0</v>
+        <v>234</v>
       </c>
       <c r="C70" s="2">
-        <v>2352.55</v>
+        <v>2352.5500000000002</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>535.0</v>
+        <v>535</v>
       </c>
       <c r="C71" s="2">
         <v>324.5</v>
@@ -1309,12 +1330,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>352.0</v>
+        <v>352</v>
       </c>
       <c r="C72" s="2">
         <v>235.99</v>
@@ -1323,12 +1344,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="B73" s="2">
-        <v>688.0</v>
+        <v>688</v>
       </c>
       <c r="C73" s="2">
         <v>235.98</v>
@@ -1337,12 +1358,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
-        <v>73.0</v>
+        <v>73</v>
       </c>
       <c r="B74" s="2">
-        <v>378.0</v>
+        <v>378</v>
       </c>
       <c r="C74" s="2">
         <v>9.99</v>
@@ -1351,21 +1372,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="75">
+    <row r="75" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="C75" s="2">
-        <v>19.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>